<commit_message>
tests gcm x statsmodels, improve generate_sample func
</commit_message>
<xml_diff>
--- a/test/benchmark/algo_evaluation.xlsx
+++ b/test/benchmark/algo_evaluation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\test\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB1656-AC47-4E4B-8BE7-AEFC1A02F87D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC9FD0A-1C9B-4686-8451-8781B2E30272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="107">
   <si>
     <t>dataset</t>
   </si>
@@ -488,6 +488,12 @@
   </si>
   <si>
     <t>[-0.0894226178, -0.116601011, 0.0438991599]</t>
+  </si>
+  <si>
+    <t>statsmodels</t>
+  </si>
+  <si>
+    <t>0.28907486</t>
   </si>
 </sst>
 </file>
@@ -798,7 +804,191 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1387,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3065,137 +3255,135 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="27" t="s">
+    <row r="27" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="27">
-        <v>250</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="J27" s="30">
+      <c r="E27" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="16">
+        <v>50</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="14">
         <v>1</v>
       </c>
-      <c r="K27" s="31">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="L27" s="31">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="M27" s="31">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="N27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" s="48">
-        <v>0.28907486999999998</v>
-      </c>
-      <c r="P27" s="48">
-        <v>7.3790670000000003E-2</v>
-      </c>
-      <c r="Q27" s="49">
-        <v>0.77539077000000001</v>
-      </c>
-      <c r="R27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="S27" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="T27" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="U27" s="32"/>
+      <c r="K27" s="15">
+        <v>0.87162667000000005</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" s="18">
+        <v>0.87162667000000005</v>
+      </c>
+      <c r="P27" s="18">
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="Q27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T27" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U27" s="24"/>
     </row>
-    <row r="28" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="55" t="s">
+      <c r="C28" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="33" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="F28" s="16">
-        <v>250</v>
-      </c>
-      <c r="G28" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="33" t="s">
         <v>38</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="22" t="s">
-        <v>76</v>
+      <c r="I28" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="J28" s="14">
         <v>1</v>
       </c>
       <c r="K28" s="15">
-        <v>0.28899999999999998</v>
+        <v>0.87162667000000005</v>
       </c>
       <c r="L28" s="15">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="M28" s="15">
-        <v>0.77500000000000002</v>
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="N28" s="55" t="s">
         <v>14</v>
       </c>
       <c r="O28" s="18">
-        <v>0.28907732000000003</v>
+        <v>0.87162719</v>
       </c>
       <c r="P28" s="18">
-        <v>7.3785790000000004E-2</v>
-      </c>
-      <c r="Q28" s="56">
-        <v>0.77539374999999999</v>
-      </c>
-      <c r="R28" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="S28" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T28" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="U28" s="61" t="s">
-        <v>101</v>
-      </c>
+        <v>0.55798128000000002</v>
+      </c>
+      <c r="Q28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T28" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U28" s="24"/>
     </row>
-    <row r="29" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>52</v>
@@ -3203,7 +3391,7 @@
       <c r="C29" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="27" t="s">
@@ -3212,55 +3400,53 @@
       <c r="F29" s="27">
         <v>250</v>
       </c>
-      <c r="G29" s="47" t="s">
+      <c r="G29" s="26" t="s">
         <v>38</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="28" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="J29" s="30">
-        <v>2</v>
-      </c>
-      <c r="K29" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="L29" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="M29" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="N29" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="P29" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q29" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="R29" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="S29" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="T29" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="U29" s="53" t="s">
-        <v>65</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K29" s="31">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="L29" s="31">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M29" s="31">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="48">
+        <v>0.28907486999999998</v>
+      </c>
+      <c r="P29" s="48">
+        <v>7.3790670000000003E-2</v>
+      </c>
+      <c r="Q29" s="49">
+        <v>0.77539077000000001</v>
+      </c>
+      <c r="R29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="T29" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="U29" s="32"/>
     </row>
     <row r="30" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>90</v>
@@ -3280,216 +3466,576 @@
       <c r="G30" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" s="14">
+        <v>1</v>
+      </c>
+      <c r="K30" s="15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="L30" s="15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M30" s="15">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N30" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O30" s="18">
+        <v>0.28907732000000003</v>
+      </c>
+      <c r="P30" s="18">
+        <v>7.3785790000000004E-2</v>
+      </c>
+      <c r="Q30" s="56">
+        <v>0.77539374999999999</v>
+      </c>
+      <c r="R30" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S30" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T30" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U30" s="61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="16">
+        <v>250</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="14">
+        <v>1</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L31" s="15">
+        <v>7.3790649999999999E-2</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0.77539075999999996</v>
+      </c>
+      <c r="N31" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O31" s="18">
+        <v>0.28907732000000003</v>
+      </c>
+      <c r="P31" s="18">
+        <v>7.3785790000000004E-2</v>
+      </c>
+      <c r="Q31" s="56">
+        <v>0.77539374999999999</v>
+      </c>
+      <c r="R31" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S31" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T31" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U31" s="35"/>
+    </row>
+    <row r="32" spans="1:21" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="16">
+        <v>250</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J32" s="14">
+        <v>1</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L32" s="15">
+        <v>7.3790649999999999E-2</v>
+      </c>
+      <c r="M32" s="15">
+        <v>0.77539075999999996</v>
+      </c>
+      <c r="N32" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" s="18">
+        <v>0.28907732000000003</v>
+      </c>
+      <c r="P32" s="18">
+        <v>7.3785790000000004E-2</v>
+      </c>
+      <c r="Q32" s="56">
+        <v>0.77539374999999999</v>
+      </c>
+      <c r="R32" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S32" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U32" s="35"/>
+    </row>
+    <row r="33" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="27">
+        <v>250</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="20" t="s">
+      <c r="I33" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="57">
+      <c r="J33" s="30">
         <v>2</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K33" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L33" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="M30" s="15" t="s">
+      <c r="M33" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="N30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O30" s="38" t="s">
+      <c r="N33" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O33" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="P33" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q33" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="R33" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="S33" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="T33" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="16">
+        <v>250</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="57">
+        <v>2</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="P30" s="38" t="s">
+      <c r="P34" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="Q30" s="38" t="s">
+      <c r="Q34" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="R30" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="S30" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="T30" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="U30" s="24" t="s">
+      <c r="R34" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S34" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="T34" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="U34" s="24" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H30:H1048576 I28 H19:H22 H1:H3 H12:H17 H7:H8 H24:H28 H5 H10">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+  <conditionalFormatting sqref="H34:H1048576 I30 H19:H22 H1:H3 H12:H17 H7:H8 H24:H26 H5 H10 H29:H30">
+    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D1048576 G31:G1048576 G19:G22 G1:G3 D1:D3 G12:G17 G7:G8 D7:D8 D24:D28 G24:G28 D5 G5 D10:D22 G10">
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+  <conditionalFormatting sqref="D35:D1048576 G35:G1048576 G19:G22 G1:G3 D1:D3 G12:G17 G7:G8 D7:D8 D24:D26 G24:G26 D5 G5 D10:D22 G10 D29:D30 G29:G30">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D1048576 D1:D3 D7:D8 D24:D28 D5 D10:D22">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+  <conditionalFormatting sqref="D35:D1048576 D1:D3 D7:D8 D24:D26 D5 D10:D22 D29:D30">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+  <conditionalFormatting sqref="H33">
+    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H29)))</formula>
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G29 D29">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+  <conditionalFormatting sqref="G33 D33">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
+  <conditionalFormatting sqref="D33">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
       <formula>"no"</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34 D34">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6 D6">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="43" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23 D23">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4 D4">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N/A",H9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("yes",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30 D30">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+  <conditionalFormatting sqref="G9 D9">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H6)))</formula>
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6 D6">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+  <conditionalFormatting sqref="H31:I31">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H11)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H23)))</formula>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23 D23">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
-      <formula>"NOT OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
+  <conditionalFormatting sqref="D28">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H4)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4 D4">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="D32">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="D32">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting sqref="H32:I32">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H9)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9 D9">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NOT OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improve convergence time in LCGA
</commit_message>
<xml_diff>
--- a/test/benchmark/algo_evaluation.xlsx
+++ b/test/benchmark/algo_evaluation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\test\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\longitudinalmodels\test\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C313FF0E-D99D-49FB-950A-35384E338627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D19FA9B-0A95-456C-BEB5-1683C7574CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GCM" sheetId="1" r:id="rId1"/>
-    <sheet name="color legend" sheetId="2" r:id="rId2"/>
+    <sheet name="LCGA" sheetId="3" r:id="rId2"/>
+    <sheet name="color legend" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1653,9 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4202,6 +4201,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8268F70C-554B-428E-A076-2E8CB2A8BBC7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2EDB0-6F22-4FB8-BAC6-46632BF44A49}">
   <dimension ref="A1:A6"/>
   <sheetViews>

</xml_diff>